<commit_message>
Finish BOM v1. Add system diagram v1.
</commit_message>
<xml_diff>
--- a/sinking-clock-BOM-v1.xlsx
+++ b/sinking-clock-BOM-v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lab\sinking-clock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73432C3B-6C2B-48BA-A256-1F28EFC4971E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628DFFFB-0A5F-4F63-8036-A00FDDC57365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="109">
   <si>
     <t>Quantity</t>
   </si>
@@ -190,6 +190,177 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/kemet/C731U222MZWDAA7317/17838303</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8SOIC adapter board </t>
+  </si>
+  <si>
+    <t>Aries Electronics</t>
+  </si>
+  <si>
+    <t>LCQT-SOIC8-8</t>
+  </si>
+  <si>
+    <t>A880AR-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/aries-electronics/LCQT-SOIC8-8/4754588</t>
+  </si>
+  <si>
+    <t>Red LEDs - TH</t>
+  </si>
+  <si>
+    <t>Würth Elektronik</t>
+  </si>
+  <si>
+    <t>151031SS04000</t>
+  </si>
+  <si>
+    <t>732-5005-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/w%C3%BCrth-elektronik/151031SS04000/4489979</t>
+  </si>
+  <si>
+    <t>Buzzer - option 1</t>
+  </si>
+  <si>
+    <t>Buzzer - option 2</t>
+  </si>
+  <si>
+    <t>Buzzer - option 3</t>
+  </si>
+  <si>
+    <t>Murata Electronics</t>
+  </si>
+  <si>
+    <t>PKM22EPPH2001-B0</t>
+  </si>
+  <si>
+    <t>490-4691-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/murata-electronics/PKM22EPPH2001-B0/1219322</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/murata-electronics/PKM13EPYH4002-B0/1219328</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/cui-devices/CMI-9605IC-0380T/11674180</t>
+  </si>
+  <si>
+    <t>PKM13EPYH4002-B0</t>
+  </si>
+  <si>
+    <t>490-4697-ND</t>
+  </si>
+  <si>
+    <t>CUI Devices</t>
+  </si>
+  <si>
+    <t>CMI-9605IC-0380T</t>
+  </si>
+  <si>
+    <t>2223-CMI-9605IC-0380T-ND</t>
+  </si>
+  <si>
+    <t>USB A Male to micro B male cable</t>
+  </si>
+  <si>
+    <t>Assmann WSW Components</t>
+  </si>
+  <si>
+    <t>AK67421-0.3-VM</t>
+  </si>
+  <si>
+    <t>AE11229-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/assmann-wsw-components/AK67421-0-3-VM/5428793</t>
+  </si>
+  <si>
+    <t>IO Expanding LED Driver - 24 TSSOP</t>
+  </si>
+  <si>
+    <t>NXP USA Inc.</t>
+  </si>
+  <si>
+    <t>Barrel Jack - breadboard adapter</t>
+  </si>
+  <si>
+    <t>Chip Quik Inc.</t>
+  </si>
+  <si>
+    <t>CN0020</t>
+  </si>
+  <si>
+    <t>CN0020-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/chip-quik-inc./CN0020/5978267</t>
+  </si>
+  <si>
+    <t>120VAC-12VDC adapter</t>
+  </si>
+  <si>
+    <t>XP Power</t>
+  </si>
+  <si>
+    <t>ACM18US12</t>
+  </si>
+  <si>
+    <t>1470-3950-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/xp-power/ACM18US12/6595122</t>
+  </si>
+  <si>
+    <t>PCA9532PW,118</t>
+  </si>
+  <si>
+    <t>568-11909-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/nxp-usa-inc/PCA9532PW-118/1157036</t>
+  </si>
+  <si>
+    <t>TSSOP to DIP adapter board (28P)</t>
+  </si>
+  <si>
+    <t>Adafruit Industries LLC</t>
+  </si>
+  <si>
+    <t>1528-1068-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/adafruit-industries-llc/1208/5022797</t>
+  </si>
+  <si>
+    <t>7-seg display driver IC</t>
+  </si>
+  <si>
+    <t>Analog Devices Inc./Maxim Integrated</t>
+  </si>
+  <si>
+    <t>MAX6958AAEE+T</t>
+  </si>
+  <si>
+    <t>MAX6958AAEE+CT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/analog-devices-inc-maxim-integrated/MAX6958AAEE-T/1521774</t>
+  </si>
+  <si>
+    <t>QSOP to DIP adapter</t>
+  </si>
+  <si>
+    <t>PA0028</t>
+  </si>
+  <si>
+    <t>PA0028-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/chip-quik-inc/PA0028/5014737</t>
   </si>
 </sst>
 </file>
@@ -303,7 +474,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -311,9 +482,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -609,9 +779,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -625,22 +795,22 @@
     <col min="7" max="7" width="9" customWidth="1"/>
     <col min="8" max="8" width="8.88671875" style="3"/>
     <col min="9" max="9" width="17.6640625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="35.5546875" style="8" customWidth="1"/>
+    <col min="10" max="10" width="35.5546875" customWidth="1"/>
     <col min="12" max="12" width="18.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:12" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
@@ -668,7 +838,7 @@
       <c r="I2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="L2" s="5" t="s">
@@ -701,12 +871,12 @@
         <f>G3*H3</f>
         <v>10.97</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="7" t="s">
         <v>25</v>
       </c>
       <c r="L3" s="3">
         <f>SUM(I3:I51)</f>
-        <v>26.150000000000002</v>
+        <v>94.54000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -735,7 +905,7 @@
         <f t="shared" ref="I4:I67" si="0">G4*H4</f>
         <v>2.7600000000000002</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" s="7" t="s">
         <v>24</v>
       </c>
     </row>
@@ -765,7 +935,7 @@
         <f t="shared" si="0"/>
         <v>2.34</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="7" t="s">
         <v>23</v>
       </c>
     </row>
@@ -795,7 +965,7 @@
         <f t="shared" si="0"/>
         <v>0.92</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="J6" s="7" t="s">
         <v>30</v>
       </c>
     </row>
@@ -825,8 +995,12 @@
         <f t="shared" si="0"/>
         <v>2.7</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J7" s="7" t="s">
         <v>31</v>
+      </c>
+      <c r="L7" s="3">
+        <f>SUM(I2:I100)</f>
+        <v>94.54000000000002</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -855,7 +1029,7 @@
         <f t="shared" si="0"/>
         <v>4.08</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="J8" s="7" t="s">
         <v>36</v>
       </c>
     </row>
@@ -885,7 +1059,7 @@
         <f t="shared" si="0"/>
         <v>1.52</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="J9" s="7" t="s">
         <v>47</v>
       </c>
     </row>
@@ -915,137 +1089,425 @@
         <f t="shared" si="0"/>
         <v>0.86</v>
       </c>
-      <c r="J10" s="9" t="s">
+      <c r="J10" s="7" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11" s="3">
+        <v>3.03</v>
+      </c>
       <c r="I11" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.03</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12">
+        <v>60</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0.18</v>
+      </c>
       <c r="I12" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10.799999999999999</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0.73</v>
+      </c>
       <c r="I13" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.46</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0.39</v>
+      </c>
       <c r="I14" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.78</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" t="s">
+        <v>75</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15" s="3">
+        <v>1.34</v>
+      </c>
       <c r="I15" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.34</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" t="s">
+        <v>79</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16" s="3">
+        <v>2.7</v>
+      </c>
       <c r="I16" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.3">
+        <v>2.7</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" t="s">
+        <v>93</v>
+      </c>
+      <c r="E17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" t="s">
+        <v>94</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17" s="3">
+        <v>3.26</v>
+      </c>
       <c r="I17" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.3">
+        <v>6.52</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18" s="3">
+        <v>15.35</v>
+      </c>
       <c r="I18" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="9:9" x14ac:dyDescent="0.3">
+        <v>15.35</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" t="s">
+        <v>86</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19" s="3">
+        <v>5.29</v>
+      </c>
       <c r="I19" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="9:9" x14ac:dyDescent="0.3">
+        <v>5.29</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" t="s">
+        <v>97</v>
+      </c>
+      <c r="D20">
+        <v>1208</v>
+      </c>
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" t="s">
+        <v>98</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20" s="3">
+        <v>4.95</v>
+      </c>
       <c r="I20" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="9:9" x14ac:dyDescent="0.3">
+        <v>4.95</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" t="s">
+        <v>102</v>
+      </c>
+      <c r="E21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" t="s">
+        <v>103</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21" s="3">
+        <v>11.38</v>
+      </c>
       <c r="I21" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="9:9" x14ac:dyDescent="0.3">
+        <v>11.38</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" t="s">
+        <v>106</v>
+      </c>
+      <c r="E22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" t="s">
+        <v>107</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22" s="3">
+        <v>4.79</v>
+      </c>
       <c r="I22" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="9:9" x14ac:dyDescent="0.3">
+        <v>4.79</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I23" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I24" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I25" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I26" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I27" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I28" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I29" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I30" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I31" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I32" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1478,8 +1940,20 @@
     <hyperlink ref="J8" r:id="rId6" xr:uid="{DFC0ACD6-C5A7-4F5D-9778-EDE749232239}"/>
     <hyperlink ref="J9" r:id="rId7" xr:uid="{D5B88B3B-423F-4A98-8994-543CBAC72644}"/>
     <hyperlink ref="J10" r:id="rId8" xr:uid="{5933D3A3-1023-4D14-998F-C19774F4FA21}"/>
+    <hyperlink ref="J11" r:id="rId9" xr:uid="{6602C858-2C0D-4703-B9E6-E3180D357251}"/>
+    <hyperlink ref="J12" r:id="rId10" xr:uid="{EF382131-3817-447E-B926-A9F2EC21F222}"/>
+    <hyperlink ref="J13" r:id="rId11" xr:uid="{25B8D061-9D79-4A36-8973-69237BC1560A}"/>
+    <hyperlink ref="J14" r:id="rId12" xr:uid="{9DD6FFAB-1B03-4305-8657-4F6717BC701C}"/>
+    <hyperlink ref="J15" r:id="rId13" xr:uid="{CAD7993F-FC2F-40BE-9140-7573319C250D}"/>
+    <hyperlink ref="J16" r:id="rId14" xr:uid="{2DDD9AC5-44C4-4850-AB4E-A1032D333AC0}"/>
+    <hyperlink ref="J19" r:id="rId15" xr:uid="{DCACB9BC-1560-4946-9107-8CCB7B22AAA1}"/>
+    <hyperlink ref="J18" r:id="rId16" xr:uid="{4FA82952-2087-461D-B42B-FDDC360C0CAF}"/>
+    <hyperlink ref="J17" r:id="rId17" xr:uid="{5C8FFFC2-E30D-405C-BE08-DAAD0708D84C}"/>
+    <hyperlink ref="J20" r:id="rId18" xr:uid="{D40951A8-B477-4850-A666-80AAE047B9B8}"/>
+    <hyperlink ref="J21" r:id="rId19" xr:uid="{D16C0A33-1EF3-48F8-AADF-F2A43A710433}"/>
+    <hyperlink ref="J22" r:id="rId20" xr:uid="{F48C7229-E1E4-49C1-83BC-B7E9EE160F63}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Serial terminal sort of works. What the hell?
</commit_message>
<xml_diff>
--- a/sinking-clock-BOM-v1.xlsx
+++ b/sinking-clock-BOM-v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lab\sinking-clock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628DFFFB-0A5F-4F63-8036-A00FDDC57365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375BB08E-2151-4CEB-9AF6-570336950E96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PR-1" sheetId="1" r:id="rId1"/>
@@ -417,7 +417,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -427,6 +427,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF5050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC99FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -474,7 +504,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -490,6 +520,11 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -500,6 +535,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCC99FF"/>
       <color rgb="FFFF5050"/>
     </mruColors>
   </colors>
@@ -780,8 +816,8 @@
   <dimension ref="A1:L101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1004,7 +1040,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
+      <c r="B8" s="12" t="s">
         <v>40</v>
       </c>
       <c r="C8" t="s">
@@ -1094,7 +1130,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
+      <c r="B11" s="12" t="s">
         <v>52</v>
       </c>
       <c r="C11" t="s">
@@ -1154,7 +1190,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
+      <c r="B13" s="14" t="s">
         <v>62</v>
       </c>
       <c r="C13" t="s">
@@ -1184,7 +1220,7 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+      <c r="B14" s="14" t="s">
         <v>63</v>
       </c>
       <c r="C14" t="s">
@@ -1214,7 +1250,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
+      <c r="B15" s="15" t="s">
         <v>64</v>
       </c>
       <c r="C15" t="s">
@@ -1274,7 +1310,7 @@
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
+      <c r="B17" s="13" t="s">
         <v>81</v>
       </c>
       <c r="C17" t="s">
@@ -1364,7 +1400,7 @@
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
+      <c r="B20" s="13" t="s">
         <v>96</v>
       </c>
       <c r="C20" t="s">
@@ -1394,7 +1430,7 @@
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
+      <c r="B21" s="11" t="s">
         <v>100</v>
       </c>
       <c r="C21" t="s">
@@ -1424,7 +1460,7 @@
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
+      <c r="B22" s="11" t="s">
         <v>105</v>
       </c>
       <c r="C22" t="s">

</xml_diff>